<commit_message>
Updated `donor_id` and `tissue_id` regex to conform to SenNet IDs
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -60,7 +60,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
+          <t>SenNet ID of the source (whole organism) of the assayed tissue.</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>HuBMAP Display ID of the assayed tissue.</t>
+          <t>SenNet ID of the assayed tissue.</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Updated regex and added murine source spec
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -60,7 +60,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
+          <t>SenNet ID of the source (whole organism) of the assayed tissue.</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>HuBMAP Display ID of the assayed tissue.</t>
+          <t>SenNet ID of the assayed tissue.</t>
         </r>
       </text>
     </comment>

</xml_diff>